<commit_message>
Updating statistics for executions.
</commit_message>
<xml_diff>
--- a/output/algorithm_comparison.xlsx
+++ b/output/algorithm_comparison.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="72">
   <si>
     <t>grid_01</t>
   </si>
@@ -225,13 +225,29 @@
   </si>
   <si>
     <t>Adaptive A*</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>STDEV</t>
+  </si>
+  <si>
+    <t>RATIO  Smaller / Larger</t>
+  </si>
+  <si>
+    <t>RATIO  Backward / Forward</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -263,6 +279,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -287,7 +310,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -315,8 +338,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -325,11 +372,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -343,6 +403,18 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -356,6 +428,18 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -685,44 +769,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="5" width="9.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="9" width="9.83203125" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1">
+      <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="30">
-      <c r="A2" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>53</v>
       </c>
@@ -747,158 +836,216 @@
       <c r="I2" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3">
+        <v>2828</v>
+      </c>
+      <c r="C3">
+        <v>65</v>
+      </c>
+      <c r="D3">
+        <v>274</v>
+      </c>
+      <c r="E3">
+        <v>6.0600000000000001E-2</v>
+      </c>
+      <c r="F3">
         <v>37437</v>
       </c>
-      <c r="C3">
+      <c r="G3">
         <v>51</v>
       </c>
-      <c r="D3">
+      <c r="H3">
         <v>176</v>
       </c>
-      <c r="E3">
+      <c r="I3">
         <v>9.0800000000000006E-2</v>
       </c>
-      <c r="F3">
-        <v>2828</v>
-      </c>
-      <c r="G3">
-        <v>65</v>
-      </c>
-      <c r="H3">
-        <v>274</v>
-      </c>
-      <c r="I3">
-        <v>6.0600000000000001E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
+        <v>331</v>
+      </c>
+      <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>53</v>
+      </c>
+      <c r="E4">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="F4">
         <v>886</v>
       </c>
-      <c r="C4">
+      <c r="G4">
         <v>18</v>
       </c>
-      <c r="D4">
+      <c r="H4">
         <v>50</v>
       </c>
-      <c r="E4">
+      <c r="I4">
         <v>2.01E-2</v>
       </c>
-      <c r="F4">
-        <v>331</v>
-      </c>
-      <c r="G4">
-        <v>21</v>
-      </c>
-      <c r="H4">
-        <v>53</v>
-      </c>
-      <c r="I4">
-        <v>2.0799999999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="L4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
+        <v>60372</v>
+      </c>
+      <c r="C5">
+        <v>403</v>
+      </c>
+      <c r="D5">
+        <v>1685</v>
+      </c>
+      <c r="E5">
+        <v>0.39550000000000002</v>
+      </c>
+      <c r="F5">
         <v>423048</v>
       </c>
-      <c r="C5">
+      <c r="G5">
         <v>297</v>
       </c>
-      <c r="D5">
+      <c r="H5">
         <v>1295</v>
       </c>
-      <c r="E5">
+      <c r="I5">
         <v>0.7802</v>
       </c>
-      <c r="F5">
-        <v>60372</v>
-      </c>
-      <c r="G5">
-        <v>403</v>
-      </c>
-      <c r="H5">
-        <v>1685</v>
-      </c>
-      <c r="I5">
-        <v>0.39550000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
+        <v>1937</v>
+      </c>
+      <c r="C6">
+        <v>70</v>
+      </c>
+      <c r="D6">
+        <v>264</v>
+      </c>
+      <c r="E6">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="F6">
         <v>9777</v>
       </c>
-      <c r="C6">
+      <c r="G6">
         <v>82</v>
       </c>
-      <c r="D6">
+      <c r="H6">
         <v>258</v>
       </c>
-      <c r="E6">
+      <c r="I6">
         <v>7.5300000000000006E-2</v>
       </c>
-      <c r="F6">
-        <v>1937</v>
-      </c>
-      <c r="G6">
-        <v>70</v>
-      </c>
-      <c r="H6">
-        <v>264</v>
-      </c>
-      <c r="I6">
-        <v>6.0400000000000002E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="K6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="11">
+        <f>F54/B54</f>
+        <v>8.1698719676219689</v>
+      </c>
+      <c r="M6" s="11">
+        <f t="shared" ref="M6:O6" si="0">G54/C54</f>
+        <v>1.0184563758389262</v>
+      </c>
+      <c r="N6" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0239565587734243</v>
+      </c>
+      <c r="O6" s="11">
+        <f t="shared" si="0"/>
+        <v>1.7124422393049552</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
+        <v>1244</v>
+      </c>
+      <c r="C7">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>168</v>
+      </c>
+      <c r="E7">
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="F7">
         <v>9182</v>
       </c>
-      <c r="C7">
+      <c r="G7">
         <v>39</v>
       </c>
-      <c r="D7">
+      <c r="H7">
         <v>142</v>
       </c>
-      <c r="E7">
+      <c r="I7">
         <v>4.7E-2</v>
       </c>
-      <c r="F7">
-        <v>1244</v>
-      </c>
-      <c r="G7">
-        <v>45</v>
-      </c>
-      <c r="H7">
-        <v>168</v>
-      </c>
-      <c r="I7">
-        <v>4.7300000000000002E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="11">
+        <f>F55/B55</f>
+        <v>7.2767549537330645</v>
+      </c>
+      <c r="M7" s="11">
+        <f>G55/C55</f>
+        <v>0.99615361968892646</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" ref="N7" si="1">H55/D55</f>
+        <v>1.0375489617266169</v>
+      </c>
+      <c r="O7" s="11">
+        <f t="shared" ref="O7" si="2">I55/E55</f>
+        <v>2.351287944235481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -907,10 +1054,10 @@
         <v>5</v>
       </c>
       <c r="E8">
-        <v>5.8999999999999999E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="F8">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -919,239 +1066,239 @@
         <v>5</v>
       </c>
       <c r="I8">
-        <v>6.3E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>5.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
+        <v>1179</v>
+      </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>139</v>
+      </c>
+      <c r="E9">
+        <v>3.8899999999999997E-2</v>
+      </c>
+      <c r="F9">
         <v>1757</v>
       </c>
-      <c r="C9">
+      <c r="G9">
         <v>41</v>
       </c>
-      <c r="D9">
+      <c r="H9">
         <v>138</v>
       </c>
-      <c r="E9">
+      <c r="I9">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="F9">
-        <v>1179</v>
-      </c>
-      <c r="G9">
-        <v>40</v>
-      </c>
-      <c r="H9">
-        <v>139</v>
-      </c>
-      <c r="I9">
-        <v>3.8899999999999997E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
+        <v>2353</v>
+      </c>
+      <c r="C10">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>258</v>
+      </c>
+      <c r="E10">
+        <v>5.7099999999999998E-2</v>
+      </c>
+      <c r="F10">
         <v>6521</v>
       </c>
-      <c r="C10">
+      <c r="G10">
         <v>65</v>
       </c>
-      <c r="D10">
+      <c r="H10">
         <v>229</v>
       </c>
-      <c r="E10">
+      <c r="I10">
         <v>5.8500000000000003E-2</v>
       </c>
-      <c r="F10">
-        <v>2353</v>
-      </c>
-      <c r="G10">
-        <v>62</v>
-      </c>
-      <c r="H10">
-        <v>258</v>
-      </c>
-      <c r="I10">
-        <v>5.7099999999999998E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11">
+        <v>1358</v>
+      </c>
+      <c r="C11">
+        <v>51</v>
+      </c>
+      <c r="D11">
+        <v>190</v>
+      </c>
+      <c r="E11">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F11">
         <v>5874</v>
       </c>
-      <c r="C11">
+      <c r="G11">
         <v>53</v>
       </c>
-      <c r="D11">
+      <c r="H11">
         <v>184</v>
       </c>
-      <c r="E11">
+      <c r="I11">
         <v>5.3199999999999997E-2</v>
       </c>
-      <c r="F11">
-        <v>1358</v>
-      </c>
-      <c r="G11">
-        <v>51</v>
-      </c>
-      <c r="H11">
-        <v>190</v>
-      </c>
-      <c r="I11">
-        <v>4.4999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12">
+        <v>556</v>
+      </c>
+      <c r="C12">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>86</v>
+      </c>
+      <c r="E12">
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="F12">
         <v>1754</v>
       </c>
-      <c r="C12">
+      <c r="G12">
         <v>26</v>
       </c>
-      <c r="D12">
+      <c r="H12">
         <v>88</v>
       </c>
-      <c r="E12">
+      <c r="I12">
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="F12">
-        <v>556</v>
-      </c>
-      <c r="G12">
-        <v>24</v>
-      </c>
-      <c r="H12">
-        <v>86</v>
-      </c>
-      <c r="I12">
-        <v>2.2100000000000002E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13">
+        <v>91767</v>
+      </c>
+      <c r="C13">
+        <v>206</v>
+      </c>
+      <c r="D13">
+        <v>947</v>
+      </c>
+      <c r="E13">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="F13">
         <v>121578</v>
       </c>
-      <c r="C13">
+      <c r="G13">
         <v>219</v>
       </c>
-      <c r="D13">
+      <c r="H13">
         <v>958</v>
       </c>
-      <c r="E13">
+      <c r="I13">
         <v>0.32169999999999999</v>
       </c>
-      <c r="F13">
-        <v>91767</v>
-      </c>
-      <c r="G13">
-        <v>206</v>
-      </c>
-      <c r="H13">
-        <v>947</v>
-      </c>
-      <c r="I13">
-        <v>0.28699999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14">
+        <v>6417</v>
+      </c>
+      <c r="C14">
+        <v>118</v>
+      </c>
+      <c r="D14">
+        <v>461</v>
+      </c>
+      <c r="E14">
+        <v>0.108</v>
+      </c>
+      <c r="F14">
         <v>48708</v>
       </c>
-      <c r="C14">
+      <c r="G14">
         <v>87</v>
       </c>
-      <c r="D14">
+      <c r="H14">
         <v>300</v>
       </c>
-      <c r="E14">
+      <c r="I14">
         <v>0.1333</v>
       </c>
-      <c r="F14">
-        <v>6417</v>
-      </c>
-      <c r="G14">
-        <v>118</v>
-      </c>
-      <c r="H14">
-        <v>461</v>
-      </c>
-      <c r="I14">
-        <v>0.108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15">
+        <v>12108</v>
+      </c>
+      <c r="C15">
+        <v>175</v>
+      </c>
+      <c r="D15">
+        <v>730</v>
+      </c>
+      <c r="E15">
+        <v>0.15479999999999999</v>
+      </c>
+      <c r="F15">
         <v>107150</v>
       </c>
-      <c r="C15">
+      <c r="G15">
         <v>184</v>
       </c>
-      <c r="D15">
+      <c r="H15">
         <v>733</v>
       </c>
-      <c r="E15">
+      <c r="I15">
         <v>0.2727</v>
       </c>
-      <c r="F15">
-        <v>12108</v>
-      </c>
-      <c r="G15">
-        <v>175</v>
-      </c>
-      <c r="H15">
-        <v>730</v>
-      </c>
-      <c r="I15">
-        <v>0.15479999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16">
+        <v>448</v>
+      </c>
+      <c r="C16">
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <v>88</v>
+      </c>
+      <c r="E16">
+        <v>2.63E-2</v>
+      </c>
+      <c r="F16">
         <v>1234</v>
       </c>
-      <c r="C16">
+      <c r="G16">
         <v>18</v>
       </c>
-      <c r="D16">
+      <c r="H16">
         <v>70</v>
       </c>
-      <c r="E16">
+      <c r="I16">
         <v>1.9800000000000002E-2</v>
-      </c>
-      <c r="F16">
-        <v>448</v>
-      </c>
-      <c r="G16">
-        <v>26</v>
-      </c>
-      <c r="H16">
-        <v>88</v>
-      </c>
-      <c r="I16">
-        <v>2.63E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1159,28 +1306,28 @@
         <v>14</v>
       </c>
       <c r="B17">
+        <v>4373</v>
+      </c>
+      <c r="C17">
+        <v>93</v>
+      </c>
+      <c r="D17">
+        <v>382</v>
+      </c>
+      <c r="E17">
+        <v>8.6199999999999999E-2</v>
+      </c>
+      <c r="F17">
         <v>35493</v>
       </c>
-      <c r="C17">
+      <c r="G17">
         <v>81</v>
       </c>
-      <c r="D17">
+      <c r="H17">
         <v>316</v>
       </c>
-      <c r="E17">
+      <c r="I17">
         <v>0.1123</v>
-      </c>
-      <c r="F17">
-        <v>4373</v>
-      </c>
-      <c r="G17">
-        <v>93</v>
-      </c>
-      <c r="H17">
-        <v>382</v>
-      </c>
-      <c r="I17">
-        <v>8.6199999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1188,28 +1335,28 @@
         <v>15</v>
       </c>
       <c r="B18">
+        <v>3047</v>
+      </c>
+      <c r="C18">
+        <v>78</v>
+      </c>
+      <c r="D18">
+        <v>287</v>
+      </c>
+      <c r="E18">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F18">
         <v>37228</v>
       </c>
-      <c r="C18">
+      <c r="G18">
         <v>71</v>
       </c>
-      <c r="D18">
+      <c r="H18">
         <v>268</v>
       </c>
-      <c r="E18">
+      <c r="I18">
         <v>0.1047</v>
-      </c>
-      <c r="F18">
-        <v>3047</v>
-      </c>
-      <c r="G18">
-        <v>78</v>
-      </c>
-      <c r="H18">
-        <v>287</v>
-      </c>
-      <c r="I18">
-        <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1217,28 +1364,28 @@
         <v>16</v>
       </c>
       <c r="B19">
+        <v>2824</v>
+      </c>
+      <c r="C19">
+        <v>67</v>
+      </c>
+      <c r="D19">
+        <v>264</v>
+      </c>
+      <c r="E19">
+        <v>6.2399999999999997E-2</v>
+      </c>
+      <c r="F19">
         <v>10914</v>
       </c>
-      <c r="C19">
+      <c r="G19">
         <v>74</v>
       </c>
-      <c r="D19">
+      <c r="H19">
         <v>281</v>
       </c>
-      <c r="E19">
+      <c r="I19">
         <v>7.3499999999999996E-2</v>
-      </c>
-      <c r="F19">
-        <v>2824</v>
-      </c>
-      <c r="G19">
-        <v>67</v>
-      </c>
-      <c r="H19">
-        <v>264</v>
-      </c>
-      <c r="I19">
-        <v>6.2399999999999997E-2</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1246,28 +1393,28 @@
         <v>17</v>
       </c>
       <c r="B20">
+        <v>8757</v>
+      </c>
+      <c r="C20">
+        <v>126</v>
+      </c>
+      <c r="D20">
+        <v>517</v>
+      </c>
+      <c r="E20">
+        <v>0.13539999999999999</v>
+      </c>
+      <c r="F20">
         <v>198926</v>
       </c>
-      <c r="C20">
+      <c r="G20">
         <v>162</v>
       </c>
-      <c r="D20">
+      <c r="H20">
         <v>691</v>
       </c>
-      <c r="E20">
+      <c r="I20">
         <v>0.38940000000000002</v>
-      </c>
-      <c r="F20">
-        <v>8757</v>
-      </c>
-      <c r="G20">
-        <v>126</v>
-      </c>
-      <c r="H20">
-        <v>517</v>
-      </c>
-      <c r="I20">
-        <v>0.13539999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1275,28 +1422,28 @@
         <v>18</v>
       </c>
       <c r="B21">
+        <v>5024</v>
+      </c>
+      <c r="C21">
+        <v>118</v>
+      </c>
+      <c r="D21">
+        <v>488</v>
+      </c>
+      <c r="E21">
+        <v>0.10340000000000001</v>
+      </c>
+      <c r="F21">
         <v>31212</v>
       </c>
-      <c r="C21">
+      <c r="G21">
         <v>126</v>
       </c>
-      <c r="D21">
+      <c r="H21">
         <v>518</v>
       </c>
-      <c r="E21">
+      <c r="I21">
         <v>0.1305</v>
-      </c>
-      <c r="F21">
-        <v>5024</v>
-      </c>
-      <c r="G21">
-        <v>118</v>
-      </c>
-      <c r="H21">
-        <v>488</v>
-      </c>
-      <c r="I21">
-        <v>0.10340000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1304,28 +1451,28 @@
         <v>19</v>
       </c>
       <c r="B22">
+        <v>3564</v>
+      </c>
+      <c r="C22">
+        <v>88</v>
+      </c>
+      <c r="D22">
+        <v>384</v>
+      </c>
+      <c r="E22">
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="F22">
         <v>22527</v>
       </c>
-      <c r="C22">
+      <c r="G22">
         <v>94</v>
       </c>
-      <c r="D22">
+      <c r="H22">
         <v>402</v>
       </c>
-      <c r="E22">
+      <c r="I22">
         <v>0.1024</v>
-      </c>
-      <c r="F22">
-        <v>3564</v>
-      </c>
-      <c r="G22">
-        <v>88</v>
-      </c>
-      <c r="H22">
-        <v>384</v>
-      </c>
-      <c r="I22">
-        <v>8.1900000000000001E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1333,28 +1480,28 @@
         <v>20</v>
       </c>
       <c r="B23">
+        <v>2485</v>
+      </c>
+      <c r="C23">
+        <v>80</v>
+      </c>
+      <c r="D23">
+        <v>317</v>
+      </c>
+      <c r="E23">
+        <v>7.0499999999999993E-2</v>
+      </c>
+      <c r="F23">
         <v>18660</v>
       </c>
-      <c r="C23">
+      <c r="G23">
         <v>101</v>
       </c>
-      <c r="D23">
+      <c r="H23">
         <v>460</v>
       </c>
-      <c r="E23">
+      <c r="I23">
         <v>0.1007</v>
-      </c>
-      <c r="F23">
-        <v>2485</v>
-      </c>
-      <c r="G23">
-        <v>80</v>
-      </c>
-      <c r="H23">
-        <v>317</v>
-      </c>
-      <c r="I23">
-        <v>7.0499999999999993E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1362,28 +1509,28 @@
         <v>21</v>
       </c>
       <c r="B24">
+        <v>1777</v>
+      </c>
+      <c r="C24">
+        <v>47</v>
+      </c>
+      <c r="D24">
+        <v>189</v>
+      </c>
+      <c r="E24">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="F24">
         <v>3834</v>
       </c>
-      <c r="C24">
+      <c r="G24">
         <v>50</v>
       </c>
-      <c r="D24">
+      <c r="H24">
         <v>224</v>
       </c>
-      <c r="E24">
+      <c r="I24">
         <v>4.7399999999999998E-2</v>
-      </c>
-      <c r="F24">
-        <v>1777</v>
-      </c>
-      <c r="G24">
-        <v>47</v>
-      </c>
-      <c r="H24">
-        <v>189</v>
-      </c>
-      <c r="I24">
-        <v>4.0300000000000002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1391,28 +1538,28 @@
         <v>22</v>
       </c>
       <c r="B25">
+        <v>481</v>
+      </c>
+      <c r="C25">
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <v>110</v>
+      </c>
+      <c r="E25">
+        <v>2.4899999999999999E-2</v>
+      </c>
+      <c r="F25">
         <v>1493</v>
       </c>
-      <c r="C25">
+      <c r="G25">
         <v>27</v>
       </c>
-      <c r="D25">
+      <c r="H25">
         <v>104</v>
       </c>
-      <c r="E25">
+      <c r="I25">
         <v>2.29E-2</v>
-      </c>
-      <c r="F25">
-        <v>481</v>
-      </c>
-      <c r="G25">
-        <v>29</v>
-      </c>
-      <c r="H25">
-        <v>110</v>
-      </c>
-      <c r="I25">
-        <v>2.4899999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1420,28 +1567,28 @@
         <v>23</v>
       </c>
       <c r="B26">
+        <v>90</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>34</v>
+      </c>
+      <c r="E26">
+        <v>1.17E-2</v>
+      </c>
+      <c r="F26">
         <v>713</v>
       </c>
-      <c r="C26">
+      <c r="G26">
         <v>23</v>
       </c>
-      <c r="D26">
+      <c r="H26">
         <v>88</v>
       </c>
-      <c r="E26">
+      <c r="I26">
         <v>2.3400000000000001E-2</v>
-      </c>
-      <c r="F26">
-        <v>90</v>
-      </c>
-      <c r="G26">
-        <v>9</v>
-      </c>
-      <c r="H26">
-        <v>34</v>
-      </c>
-      <c r="I26">
-        <v>1.17E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1449,28 +1596,28 @@
         <v>24</v>
       </c>
       <c r="B27">
+        <v>4837</v>
+      </c>
+      <c r="C27">
+        <v>93</v>
+      </c>
+      <c r="D27">
+        <v>306</v>
+      </c>
+      <c r="E27">
+        <v>8.8300000000000003E-2</v>
+      </c>
+      <c r="F27">
         <v>19222</v>
       </c>
-      <c r="C27">
+      <c r="G27">
         <v>86</v>
       </c>
-      <c r="D27">
+      <c r="H27">
         <v>273</v>
       </c>
-      <c r="E27">
+      <c r="I27">
         <v>9.4200000000000006E-2</v>
-      </c>
-      <c r="F27">
-        <v>4837</v>
-      </c>
-      <c r="G27">
-        <v>93</v>
-      </c>
-      <c r="H27">
-        <v>306</v>
-      </c>
-      <c r="I27">
-        <v>8.8300000000000003E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1478,28 +1625,28 @@
         <v>25</v>
       </c>
       <c r="B28">
+        <v>1125</v>
+      </c>
+      <c r="C28">
+        <v>38</v>
+      </c>
+      <c r="D28">
+        <v>159</v>
+      </c>
+      <c r="E28">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F28">
         <v>2108</v>
       </c>
-      <c r="C28">
+      <c r="G28">
         <v>41</v>
       </c>
-      <c r="D28">
+      <c r="H28">
         <v>162</v>
       </c>
-      <c r="E28">
+      <c r="I28">
         <v>3.85E-2</v>
-      </c>
-      <c r="F28">
-        <v>1125</v>
-      </c>
-      <c r="G28">
-        <v>38</v>
-      </c>
-      <c r="H28">
-        <v>159</v>
-      </c>
-      <c r="I28">
-        <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1507,28 +1654,28 @@
         <v>26</v>
       </c>
       <c r="B29">
+        <v>340</v>
+      </c>
+      <c r="C29">
+        <v>25</v>
+      </c>
+      <c r="D29">
+        <v>83</v>
+      </c>
+      <c r="E29">
+        <v>2.24E-2</v>
+      </c>
+      <c r="F29">
         <v>459</v>
       </c>
-      <c r="C29">
+      <c r="G29">
         <v>24</v>
       </c>
-      <c r="D29">
+      <c r="H29">
         <v>82</v>
       </c>
-      <c r="E29">
+      <c r="I29">
         <v>2.2800000000000001E-2</v>
-      </c>
-      <c r="F29">
-        <v>340</v>
-      </c>
-      <c r="G29">
-        <v>25</v>
-      </c>
-      <c r="H29">
-        <v>83</v>
-      </c>
-      <c r="I29">
-        <v>2.24E-2</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1536,28 +1683,28 @@
         <v>27</v>
       </c>
       <c r="B30">
+        <v>8433</v>
+      </c>
+      <c r="C30">
+        <v>135</v>
+      </c>
+      <c r="D30">
+        <v>510</v>
+      </c>
+      <c r="E30">
+        <v>0.1278</v>
+      </c>
+      <c r="F30">
         <v>68775</v>
       </c>
-      <c r="C30">
+      <c r="G30">
         <v>126</v>
       </c>
-      <c r="D30">
+      <c r="H30">
         <v>511</v>
       </c>
-      <c r="E30">
+      <c r="I30">
         <v>0.17860000000000001</v>
-      </c>
-      <c r="F30">
-        <v>8433</v>
-      </c>
-      <c r="G30">
-        <v>135</v>
-      </c>
-      <c r="H30">
-        <v>510</v>
-      </c>
-      <c r="I30">
-        <v>0.1278</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1565,28 +1712,28 @@
         <v>28</v>
       </c>
       <c r="B31">
+        <v>486</v>
+      </c>
+      <c r="C31">
+        <v>24</v>
+      </c>
+      <c r="D31">
+        <v>91</v>
+      </c>
+      <c r="E31">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="F31">
         <v>2255</v>
       </c>
-      <c r="C31">
+      <c r="G31">
         <v>28</v>
       </c>
-      <c r="D31">
+      <c r="H31">
         <v>105</v>
       </c>
-      <c r="E31">
+      <c r="I31">
         <v>2.9399999999999999E-2</v>
-      </c>
-      <c r="F31">
-        <v>486</v>
-      </c>
-      <c r="G31">
-        <v>24</v>
-      </c>
-      <c r="H31">
-        <v>91</v>
-      </c>
-      <c r="I31">
-        <v>2.4500000000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1594,28 +1741,28 @@
         <v>29</v>
       </c>
       <c r="B32">
+        <v>1087</v>
+      </c>
+      <c r="C32">
+        <v>36</v>
+      </c>
+      <c r="D32">
+        <v>159</v>
+      </c>
+      <c r="E32">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F32">
         <v>6177</v>
       </c>
-      <c r="C32">
+      <c r="G32">
         <v>39</v>
       </c>
-      <c r="D32">
+      <c r="H32">
         <v>162</v>
       </c>
-      <c r="E32">
+      <c r="I32">
         <v>4.2799999999999998E-2</v>
-      </c>
-      <c r="F32">
-        <v>1087</v>
-      </c>
-      <c r="G32">
-        <v>36</v>
-      </c>
-      <c r="H32">
-        <v>159</v>
-      </c>
-      <c r="I32">
-        <v>3.1E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1623,28 +1770,28 @@
         <v>30</v>
       </c>
       <c r="B33">
+        <v>26045</v>
+      </c>
+      <c r="C33">
+        <v>255</v>
+      </c>
+      <c r="D33">
+        <v>999</v>
+      </c>
+      <c r="E33">
+        <v>0.2727</v>
+      </c>
+      <c r="F33">
         <v>464875</v>
       </c>
-      <c r="C33">
+      <c r="G33">
         <v>259</v>
       </c>
-      <c r="D33">
+      <c r="H33">
         <v>961</v>
       </c>
-      <c r="E33">
+      <c r="I33">
         <v>0.76659999999999995</v>
-      </c>
-      <c r="F33">
-        <v>26045</v>
-      </c>
-      <c r="G33">
-        <v>255</v>
-      </c>
-      <c r="H33">
-        <v>999</v>
-      </c>
-      <c r="I33">
-        <v>0.2727</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1652,28 +1799,28 @@
         <v>31</v>
       </c>
       <c r="B34">
+        <v>10729</v>
+      </c>
+      <c r="C34">
+        <v>175</v>
+      </c>
+      <c r="D34">
+        <v>606</v>
+      </c>
+      <c r="E34">
+        <v>0.17560000000000001</v>
+      </c>
+      <c r="F34">
         <v>148069</v>
       </c>
-      <c r="C34">
+      <c r="G34">
         <v>157</v>
       </c>
-      <c r="D34">
+      <c r="H34">
         <v>560</v>
       </c>
-      <c r="E34">
+      <c r="I34">
         <v>0.30590000000000001</v>
-      </c>
-      <c r="F34">
-        <v>10729</v>
-      </c>
-      <c r="G34">
-        <v>175</v>
-      </c>
-      <c r="H34">
-        <v>606</v>
-      </c>
-      <c r="I34">
-        <v>0.17560000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1681,28 +1828,28 @@
         <v>32</v>
       </c>
       <c r="B35">
+        <v>1169</v>
+      </c>
+      <c r="C35">
+        <v>45</v>
+      </c>
+      <c r="D35">
+        <v>141</v>
+      </c>
+      <c r="E35">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="F35">
         <v>8734</v>
       </c>
-      <c r="C35">
+      <c r="G35">
         <v>38</v>
       </c>
-      <c r="D35">
+      <c r="H35">
         <v>126</v>
       </c>
-      <c r="E35">
+      <c r="I35">
         <v>4.6399999999999997E-2</v>
-      </c>
-      <c r="F35">
-        <v>1169</v>
-      </c>
-      <c r="G35">
-        <v>45</v>
-      </c>
-      <c r="H35">
-        <v>141</v>
-      </c>
-      <c r="I35">
-        <v>4.3099999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1710,28 +1857,28 @@
         <v>33</v>
       </c>
       <c r="B36">
+        <v>1514</v>
+      </c>
+      <c r="C36">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <v>138</v>
+      </c>
+      <c r="E36">
+        <v>3.8800000000000001E-2</v>
+      </c>
+      <c r="F36">
         <v>16786</v>
       </c>
-      <c r="C36">
+      <c r="G36">
         <v>45</v>
       </c>
-      <c r="D36">
+      <c r="H36">
         <v>149</v>
       </c>
-      <c r="E36">
+      <c r="I36">
         <v>5.67E-2</v>
-      </c>
-      <c r="F36">
-        <v>1514</v>
-      </c>
-      <c r="G36">
-        <v>38</v>
-      </c>
-      <c r="H36">
-        <v>138</v>
-      </c>
-      <c r="I36">
-        <v>3.8800000000000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1739,28 +1886,28 @@
         <v>34</v>
       </c>
       <c r="B37">
+        <v>1359</v>
+      </c>
+      <c r="C37">
+        <v>43</v>
+      </c>
+      <c r="D37">
+        <v>159</v>
+      </c>
+      <c r="E37">
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="F37">
         <v>11550</v>
       </c>
-      <c r="C37">
+      <c r="G37">
         <v>36</v>
       </c>
-      <c r="D37">
+      <c r="H37">
         <v>136</v>
       </c>
-      <c r="E37">
+      <c r="I37">
         <v>4.1300000000000003E-2</v>
-      </c>
-      <c r="F37">
-        <v>1359</v>
-      </c>
-      <c r="G37">
-        <v>43</v>
-      </c>
-      <c r="H37">
-        <v>159</v>
-      </c>
-      <c r="I37">
-        <v>4.7399999999999998E-2</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1768,28 +1915,28 @@
         <v>35</v>
       </c>
       <c r="B38">
+        <v>108</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>34</v>
+      </c>
+      <c r="E38">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="F38">
         <v>564</v>
       </c>
-      <c r="C38">
+      <c r="G38">
         <v>9</v>
       </c>
-      <c r="D38">
+      <c r="H38">
         <v>36</v>
       </c>
-      <c r="E38">
+      <c r="I38">
         <v>9.1000000000000004E-3</v>
-      </c>
-      <c r="F38">
-        <v>108</v>
-      </c>
-      <c r="G38">
-        <v>7</v>
-      </c>
-      <c r="H38">
-        <v>34</v>
-      </c>
-      <c r="I38">
-        <v>9.2999999999999992E-3</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1797,28 +1944,28 @@
         <v>36</v>
       </c>
       <c r="B39">
+        <v>30112</v>
+      </c>
+      <c r="C39">
+        <v>203</v>
+      </c>
+      <c r="D39">
+        <v>771</v>
+      </c>
+      <c r="E39">
+        <v>0.2273</v>
+      </c>
+      <c r="F39">
         <v>107542</v>
       </c>
-      <c r="C39">
+      <c r="G39">
         <v>191</v>
       </c>
-      <c r="D39">
+      <c r="H39">
         <v>719</v>
       </c>
-      <c r="E39">
+      <c r="I39">
         <v>0.2787</v>
-      </c>
-      <c r="F39">
-        <v>30112</v>
-      </c>
-      <c r="G39">
-        <v>203</v>
-      </c>
-      <c r="H39">
-        <v>771</v>
-      </c>
-      <c r="I39">
-        <v>0.2273</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1826,28 +1973,28 @@
         <v>37</v>
       </c>
       <c r="B40">
+        <v>1691</v>
+      </c>
+      <c r="C40">
+        <v>47</v>
+      </c>
+      <c r="D40">
+        <v>183</v>
+      </c>
+      <c r="E40">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="F40">
         <v>34178</v>
       </c>
-      <c r="C40">
+      <c r="G40">
         <v>85</v>
       </c>
-      <c r="D40">
+      <c r="H40">
         <v>383</v>
       </c>
-      <c r="E40">
+      <c r="I40">
         <v>0.1137</v>
-      </c>
-      <c r="F40">
-        <v>1691</v>
-      </c>
-      <c r="G40">
-        <v>47</v>
-      </c>
-      <c r="H40">
-        <v>183</v>
-      </c>
-      <c r="I40">
-        <v>3.8600000000000002E-2</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1855,28 +2002,28 @@
         <v>38</v>
       </c>
       <c r="B41">
+        <v>677</v>
+      </c>
+      <c r="C41">
+        <v>34</v>
+      </c>
+      <c r="D41">
+        <v>115</v>
+      </c>
+      <c r="E41">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="F41">
         <v>2225</v>
       </c>
-      <c r="C41">
+      <c r="G41">
         <v>35</v>
       </c>
-      <c r="D41">
+      <c r="H41">
         <v>108</v>
       </c>
-      <c r="E41">
+      <c r="I41">
         <v>3.04E-2</v>
-      </c>
-      <c r="F41">
-        <v>677</v>
-      </c>
-      <c r="G41">
-        <v>34</v>
-      </c>
-      <c r="H41">
-        <v>115</v>
-      </c>
-      <c r="I41">
-        <v>3.1399999999999997E-2</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1884,28 +2031,28 @@
         <v>39</v>
       </c>
       <c r="B42">
+        <v>36812</v>
+      </c>
+      <c r="C42">
+        <v>371</v>
+      </c>
+      <c r="D42">
+        <v>1518</v>
+      </c>
+      <c r="E42">
+        <v>0.35070000000000001</v>
+      </c>
+      <c r="F42">
         <v>468905</v>
       </c>
-      <c r="C42">
+      <c r="G42">
         <v>366</v>
       </c>
-      <c r="D42">
+      <c r="H42">
         <v>1523</v>
       </c>
-      <c r="E42">
+      <c r="I42">
         <v>0.87109999999999999</v>
-      </c>
-      <c r="F42">
-        <v>36812</v>
-      </c>
-      <c r="G42">
-        <v>371</v>
-      </c>
-      <c r="H42">
-        <v>1518</v>
-      </c>
-      <c r="I42">
-        <v>0.35070000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1913,28 +2060,28 @@
         <v>40</v>
       </c>
       <c r="B43">
+        <v>9069</v>
+      </c>
+      <c r="C43">
+        <v>153</v>
+      </c>
+      <c r="D43">
+        <v>578</v>
+      </c>
+      <c r="E43">
+        <v>0.15029999999999999</v>
+      </c>
+      <c r="F43">
         <v>132524</v>
       </c>
-      <c r="C43">
+      <c r="G43">
         <v>164</v>
       </c>
-      <c r="D43">
+      <c r="H43">
         <v>599</v>
       </c>
-      <c r="E43">
+      <c r="I43">
         <v>0.28839999999999999</v>
-      </c>
-      <c r="F43">
-        <v>9069</v>
-      </c>
-      <c r="G43">
-        <v>153</v>
-      </c>
-      <c r="H43">
-        <v>578</v>
-      </c>
-      <c r="I43">
-        <v>0.15029999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1942,28 +2089,28 @@
         <v>41</v>
       </c>
       <c r="B44">
+        <v>6714</v>
+      </c>
+      <c r="C44">
+        <v>122</v>
+      </c>
+      <c r="D44">
+        <v>479</v>
+      </c>
+      <c r="E44">
+        <v>0.113</v>
+      </c>
+      <c r="F44">
         <v>60428</v>
       </c>
-      <c r="C44">
+      <c r="G44">
         <v>82</v>
       </c>
-      <c r="D44">
+      <c r="H44">
         <v>347</v>
       </c>
-      <c r="E44">
+      <c r="I44">
         <v>0.13819999999999999</v>
-      </c>
-      <c r="F44">
-        <v>6714</v>
-      </c>
-      <c r="G44">
-        <v>122</v>
-      </c>
-      <c r="H44">
-        <v>479</v>
-      </c>
-      <c r="I44">
-        <v>0.113</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1971,28 +2118,28 @@
         <v>42</v>
       </c>
       <c r="B45">
+        <v>3374</v>
+      </c>
+      <c r="C45">
+        <v>77</v>
+      </c>
+      <c r="D45">
+        <v>256</v>
+      </c>
+      <c r="E45">
+        <v>7.7399999999999997E-2</v>
+      </c>
+      <c r="F45">
         <v>30497</v>
       </c>
-      <c r="C45">
+      <c r="G45">
         <v>104</v>
       </c>
-      <c r="D45">
+      <c r="H45">
         <v>335</v>
       </c>
-      <c r="E45">
+      <c r="I45">
         <v>0.1195</v>
-      </c>
-      <c r="F45">
-        <v>3374</v>
-      </c>
-      <c r="G45">
-        <v>77</v>
-      </c>
-      <c r="H45">
-        <v>256</v>
-      </c>
-      <c r="I45">
-        <v>7.7399999999999997E-2</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2000,28 +2147,28 @@
         <v>43</v>
       </c>
       <c r="B46">
+        <v>3314</v>
+      </c>
+      <c r="C46">
+        <v>99</v>
+      </c>
+      <c r="D46">
+        <v>401</v>
+      </c>
+      <c r="E46">
+        <v>0.1031</v>
+      </c>
+      <c r="F46">
         <v>11370</v>
       </c>
-      <c r="C46">
+      <c r="G46">
         <v>105</v>
       </c>
-      <c r="D46">
+      <c r="H46">
         <v>379</v>
       </c>
-      <c r="E46">
+      <c r="I46">
         <v>0.10249999999999999</v>
-      </c>
-      <c r="F46">
-        <v>3314</v>
-      </c>
-      <c r="G46">
-        <v>99</v>
-      </c>
-      <c r="H46">
-        <v>401</v>
-      </c>
-      <c r="I46">
-        <v>0.1031</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2029,28 +2176,28 @@
         <v>44</v>
       </c>
       <c r="B47">
+        <v>8143</v>
+      </c>
+      <c r="C47">
+        <v>114</v>
+      </c>
+      <c r="D47">
+        <v>425</v>
+      </c>
+      <c r="E47">
+        <v>0.1116</v>
+      </c>
+      <c r="F47">
         <v>30422</v>
       </c>
-      <c r="C47">
+      <c r="G47">
         <v>122</v>
       </c>
-      <c r="D47">
+      <c r="H47">
         <v>457</v>
       </c>
-      <c r="E47">
+      <c r="I47">
         <v>0.13170000000000001</v>
-      </c>
-      <c r="F47">
-        <v>8143</v>
-      </c>
-      <c r="G47">
-        <v>114</v>
-      </c>
-      <c r="H47">
-        <v>425</v>
-      </c>
-      <c r="I47">
-        <v>0.1116</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2058,28 +2205,28 @@
         <v>45</v>
       </c>
       <c r="B48">
+        <v>17694</v>
+      </c>
+      <c r="C48">
+        <v>196</v>
+      </c>
+      <c r="D48">
+        <v>847</v>
+      </c>
+      <c r="E48">
+        <v>0.191</v>
+      </c>
+      <c r="F48">
         <v>360757</v>
       </c>
-      <c r="C48">
+      <c r="G48">
         <v>194</v>
       </c>
-      <c r="D48">
+      <c r="H48">
         <v>839</v>
       </c>
-      <c r="E48">
+      <c r="I48">
         <v>0.60409999999999997</v>
-      </c>
-      <c r="F48">
-        <v>17694</v>
-      </c>
-      <c r="G48">
-        <v>196</v>
-      </c>
-      <c r="H48">
-        <v>847</v>
-      </c>
-      <c r="I48">
-        <v>0.191</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2087,28 +2234,28 @@
         <v>46</v>
       </c>
       <c r="B49">
+        <v>5227</v>
+      </c>
+      <c r="C49">
+        <v>80</v>
+      </c>
+      <c r="D49">
+        <v>303</v>
+      </c>
+      <c r="E49">
+        <v>8.09E-2</v>
+      </c>
+      <c r="F49">
         <v>30329</v>
       </c>
-      <c r="C49">
+      <c r="G49">
         <v>71</v>
       </c>
-      <c r="D49">
+      <c r="H49">
         <v>254</v>
       </c>
-      <c r="E49">
+      <c r="I49">
         <v>9.9699999999999997E-2</v>
-      </c>
-      <c r="F49">
-        <v>5227</v>
-      </c>
-      <c r="G49">
-        <v>80</v>
-      </c>
-      <c r="H49">
-        <v>303</v>
-      </c>
-      <c r="I49">
-        <v>8.09E-2</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2116,28 +2263,28 @@
         <v>47</v>
       </c>
       <c r="B50">
+        <v>592</v>
+      </c>
+      <c r="C50">
+        <v>31</v>
+      </c>
+      <c r="D50">
+        <v>112</v>
+      </c>
+      <c r="E50">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="F50">
         <v>2854</v>
       </c>
-      <c r="C50">
+      <c r="G50">
         <v>29</v>
       </c>
-      <c r="D50">
+      <c r="H50">
         <v>126</v>
       </c>
-      <c r="E50">
+      <c r="I50">
         <v>2.5499999999999998E-2</v>
-      </c>
-      <c r="F50">
-        <v>592</v>
-      </c>
-      <c r="G50">
-        <v>31</v>
-      </c>
-      <c r="H50">
-        <v>112</v>
-      </c>
-      <c r="I50">
-        <v>2.7199999999999998E-2</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2145,28 +2292,28 @@
         <v>48</v>
       </c>
       <c r="B51">
+        <v>7960</v>
+      </c>
+      <c r="C51">
+        <v>211</v>
+      </c>
+      <c r="D51">
+        <v>789</v>
+      </c>
+      <c r="E51">
+        <v>0.1893</v>
+      </c>
+      <c r="F51">
         <v>143303</v>
       </c>
-      <c r="C51">
+      <c r="G51">
         <v>352</v>
       </c>
-      <c r="D51">
+      <c r="H51">
         <v>1608</v>
       </c>
-      <c r="E51">
+      <c r="I51">
         <v>0.4491</v>
-      </c>
-      <c r="F51">
-        <v>7960</v>
-      </c>
-      <c r="G51">
-        <v>211</v>
-      </c>
-      <c r="H51">
-        <v>789</v>
-      </c>
-      <c r="I51">
-        <v>0.1893</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2174,238 +2321,313 @@
         <v>49</v>
       </c>
       <c r="B52">
+        <v>4193</v>
+      </c>
+      <c r="C52">
+        <v>72</v>
+      </c>
+      <c r="D52">
+        <v>302</v>
+      </c>
+      <c r="E52">
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="F52">
         <v>33873</v>
       </c>
-      <c r="C52">
+      <c r="G52">
         <v>76</v>
       </c>
-      <c r="D52">
+      <c r="H52">
         <v>316</v>
       </c>
-      <c r="E52">
+      <c r="I52">
         <v>0.10970000000000001</v>
       </c>
-      <c r="F52">
-        <v>4193</v>
-      </c>
-      <c r="G52">
-        <v>72</v>
-      </c>
-      <c r="H52">
-        <v>302</v>
-      </c>
-      <c r="I52">
-        <v>7.1599999999999997E-2</v>
-      </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B54" s="2">
-        <v>45</v>
-      </c>
-      <c r="C54" s="2">
-        <v>3</v>
-      </c>
-      <c r="D54" s="2">
-        <v>15</v>
-      </c>
-      <c r="E54" s="2">
-        <v>2.0999999999999999E-3</v>
-      </c>
-      <c r="F54" s="2">
-        <v>43</v>
-      </c>
-      <c r="G54" s="2">
-        <v>4</v>
-      </c>
-      <c r="H54" s="2">
-        <v>16</v>
-      </c>
-      <c r="I54" s="2">
-        <v>2.3999999999999998E-3</v>
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="9">
+        <f>AVERAGE(B3:B52)</f>
+        <v>8163.56</v>
+      </c>
+      <c r="C54" s="9">
+        <f>AVERAGE(C3:C52)</f>
+        <v>95.36</v>
+      </c>
+      <c r="D54" s="9">
+        <f>AVERAGE(D3:D52)</f>
+        <v>375.68</v>
+      </c>
+      <c r="E54" s="10">
+        <f>AVERAGE(E3:E52)</f>
+        <v>9.3922000000000019E-2</v>
+      </c>
+      <c r="F54" s="9">
+        <f>AVERAGE(F3:F52)</f>
+        <v>66695.240000000005</v>
+      </c>
+      <c r="G54" s="9">
+        <f>AVERAGE(G3:G52)</f>
+        <v>97.12</v>
+      </c>
+      <c r="H54" s="9">
+        <f t="shared" ref="H54:I54" si="3">AVERAGE(H3:H52)</f>
+        <v>384.68</v>
+      </c>
+      <c r="I54" s="10">
+        <f t="shared" si="3"/>
+        <v>0.16083600000000003</v>
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="2">
-        <v>43</v>
-      </c>
-      <c r="C55" s="2">
-        <v>5</v>
-      </c>
-      <c r="D55" s="2">
-        <v>13</v>
-      </c>
-      <c r="E55" s="2">
-        <v>3.3999999999999998E-3</v>
-      </c>
-      <c r="F55" s="2">
-        <v>29</v>
-      </c>
-      <c r="G55" s="2">
-        <v>4</v>
-      </c>
-      <c r="H55" s="2">
-        <v>12</v>
-      </c>
-      <c r="I55" s="2">
-        <v>2.3999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="2">
-        <v>10</v>
-      </c>
-      <c r="C56" s="2">
-        <v>2</v>
-      </c>
-      <c r="D56" s="2">
-        <v>9</v>
-      </c>
-      <c r="E56" s="2">
-        <v>1.4E-3</v>
-      </c>
-      <c r="F56" s="2">
-        <v>9</v>
-      </c>
-      <c r="G56" s="2">
-        <v>2</v>
-      </c>
-      <c r="H56" s="2">
-        <v>9</v>
-      </c>
-      <c r="I56" s="2">
-        <v>1.1999999999999999E-3</v>
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="9">
+        <f>_xlfn.STDEV.P(B3:B52)</f>
+        <v>16064.854043731613</v>
+      </c>
+      <c r="C55" s="9">
+        <f>_xlfn.STDEV.P(C3:C52)</f>
+        <v>84.671071801412793</v>
+      </c>
+      <c r="D55" s="9">
+        <f>_xlfn.STDEV.P(D3:D52)</f>
+        <v>350.41406592772501</v>
+      </c>
+      <c r="E55" s="10">
+        <f>_xlfn.STDEV.P(E3:E52)</f>
+        <v>8.6651131071671508E-2</v>
+      </c>
+      <c r="F55" s="9">
+        <f>_xlfn.STDEV.P(F3:F52)</f>
+        <v>116900.00624372267</v>
+      </c>
+      <c r="G55" s="9">
+        <f t="shared" ref="G55:I55" si="4">_xlfn.STDEV.P(G3:G52)</f>
+        <v>84.345394657918348</v>
+      </c>
+      <c r="H55" s="9">
+        <f t="shared" si="4"/>
+        <v>363.57175027771336</v>
+      </c>
+      <c r="I55" s="10">
+        <f t="shared" si="4"/>
+        <v>0.20374175984318973</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B57" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C57" s="2">
         <v>4</v>
       </c>
       <c r="D57" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E57" s="2">
         <v>2.3999999999999998E-3</v>
       </c>
       <c r="F57" s="2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G57" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H57" s="2">
         <v>15</v>
       </c>
       <c r="I57" s="2">
-        <v>2.3999999999999998E-3</v>
+        <v>2.0999999999999999E-3</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B58" s="2">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C58" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D58" s="2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E58" s="2">
-        <v>6.9999999999999999E-4</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="F58" s="2">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="G58" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H58" s="2">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I58" s="2">
-        <v>5.9999999999999995E-4</v>
+        <v>3.3999999999999998E-3</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B59" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C59" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D59" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E59" s="2">
-        <v>1E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="F59" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G59" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H59" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I59" s="2">
-        <v>0</v>
+        <v>1.4E-3</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="2">
+        <v>35</v>
+      </c>
+      <c r="C60" s="2">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2">
+        <v>15</v>
+      </c>
+      <c r="E60" s="2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="F60" s="2">
+        <v>42</v>
+      </c>
+      <c r="G60" s="2">
+        <v>4</v>
+      </c>
+      <c r="H60" s="2">
+        <v>15</v>
+      </c>
+      <c r="I60" s="2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2">
+        <v>2</v>
+      </c>
+      <c r="E61" s="2">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="F61" s="2">
+        <v>1</v>
+      </c>
+      <c r="G61" s="2">
+        <v>1</v>
+      </c>
+      <c r="H61" s="2">
+        <v>2</v>
+      </c>
+      <c r="I61" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0</v>
+      </c>
+      <c r="F62" s="2">
+        <v>0</v>
+      </c>
+      <c r="G62" s="2">
+        <v>0</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0</v>
+      </c>
+      <c r="I62" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B63" s="2">
+        <v>23</v>
+      </c>
+      <c r="C63" s="2">
+        <v>2</v>
+      </c>
+      <c r="D63" s="2">
+        <v>12</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F63" s="2">
         <v>26</v>
       </c>
-      <c r="C60" s="2">
+      <c r="G63" s="2">
         <v>2</v>
       </c>
-      <c r="D60" s="2">
+      <c r="H63" s="2">
         <v>12</v>
       </c>
-      <c r="E60" s="2">
+      <c r="I63" s="2">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="F60" s="2">
-        <v>23</v>
-      </c>
-      <c r="G60" s="2">
-        <v>2</v>
-      </c>
-      <c r="H60" s="2">
-        <v>12</v>
-      </c>
-      <c r="I60" s="2">
-        <v>1.1999999999999999E-3</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="L4:O4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2419,11 +2641,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2436,27 +2658,30 @@
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1">
+      <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="30">
-      <c r="A2" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2482,7 +2707,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2511,7 +2736,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2539,8 +2764,14 @@
       <c r="I4">
         <v>6.3700000000000007E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="L4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2568,8 +2799,20 @@
       <c r="I5">
         <v>4.1631999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2597,8 +2840,27 @@
       <c r="I6">
         <v>0.19789999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="K6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="11">
+        <f>F54/B54</f>
+        <v>55.845185188814682</v>
+      </c>
+      <c r="M6" s="11">
+        <f t="shared" ref="M6:O7" si="0">G54/C54</f>
+        <v>1.0102768456375839</v>
+      </c>
+      <c r="N6" s="11">
+        <f t="shared" si="0"/>
+        <v>0.99233390119250431</v>
+      </c>
+      <c r="O6" s="11">
+        <f t="shared" si="0"/>
+        <v>8.8686898559956369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2626,8 +2888,27 @@
       <c r="I7">
         <v>0.21310000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="11">
+        <f>F55/B55</f>
+        <v>40.533491693501091</v>
+      </c>
+      <c r="M7" s="11">
+        <f>G55/C55</f>
+        <v>0.87430412771404786</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="0"/>
+        <v>0.84877201707606476</v>
+      </c>
+      <c r="O7" s="11">
+        <f t="shared" si="0"/>
+        <v>12.815880593359926</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2656,7 +2937,7 @@
         <v>0.1076</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -2685,7 +2966,7 @@
         <v>9.98E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2714,7 +2995,7 @@
         <v>0.37219999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2743,7 +3024,7 @@
         <v>0.61080000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2772,7 +3053,7 @@
         <v>0.1608</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2801,7 +3082,7 @@
         <v>2.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2830,7 +3111,7 @@
         <v>0.98470000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2859,7 +3140,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3816,7 +4097,7 @@
         <v>3.0897000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -3845,7 +4126,7 @@
         <v>0.21790000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -3874,7 +4155,7 @@
         <v>3.7699999999999997E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -3903,7 +4184,7 @@
         <v>0.89670000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -3932,137 +4213,138 @@
         <v>0.98080000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="2" t="s">
+    <row r="53" spans="1:14">
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="9">
+        <f>AVERAGE(B3:B52)</f>
+        <v>8163.56</v>
+      </c>
+      <c r="C54" s="9">
+        <f t="shared" ref="C54:I54" si="1">AVERAGE(C3:C52)</f>
+        <v>95.36</v>
+      </c>
+      <c r="D54" s="9">
+        <f t="shared" si="1"/>
+        <v>375.68</v>
+      </c>
+      <c r="E54" s="10">
+        <f>AVERAGE(E3:E52)</f>
+        <v>8.7913999999999978E-2</v>
+      </c>
+      <c r="F54" s="9">
+        <f>AVERAGE(F3:F52)</f>
+        <v>455895.52</v>
+      </c>
+      <c r="G54" s="9">
+        <f t="shared" si="1"/>
+        <v>96.34</v>
+      </c>
+      <c r="H54" s="9">
+        <f t="shared" si="1"/>
+        <v>372.8</v>
+      </c>
+      <c r="I54" s="10">
+        <f>AVERAGE(I3:I52)</f>
+        <v>0.77968200000000021</v>
+      </c>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="9">
+        <f>_xlfn.STDEV.P(B3:B52)</f>
+        <v>16064.854043731613</v>
+      </c>
+      <c r="C55" s="9">
+        <f t="shared" ref="C55:I55" si="2">_xlfn.STDEV.P(C3:C52)</f>
+        <v>84.671071801412793</v>
+      </c>
+      <c r="D55" s="9">
+        <f t="shared" si="2"/>
+        <v>350.41406592772501</v>
+      </c>
+      <c r="E55" s="10">
+        <f t="shared" si="2"/>
+        <v>8.3714407386064685E-2</v>
+      </c>
+      <c r="F55" s="9">
+        <f t="shared" si="2"/>
+        <v>651164.6279389027</v>
+      </c>
+      <c r="G55" s="9">
+        <f t="shared" si="2"/>
+        <v>74.02826757394773</v>
+      </c>
+      <c r="H55" s="9">
+        <f t="shared" si="2"/>
+        <v>297.42165354930029</v>
+      </c>
+      <c r="I55" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0728738490036933</v>
+      </c>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B57" s="2">
         <v>43</v>
-      </c>
-      <c r="C54" s="2">
-        <v>4</v>
-      </c>
-      <c r="D54" s="2">
-        <v>16</v>
-      </c>
-      <c r="E54" s="2">
-        <v>2.8E-3</v>
-      </c>
-      <c r="F54" s="2">
-        <v>37</v>
-      </c>
-      <c r="G54" s="2">
-        <v>4</v>
-      </c>
-      <c r="H54" s="2">
-        <v>16</v>
-      </c>
-      <c r="I54" s="2">
-        <v>2.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="2">
-        <v>29</v>
-      </c>
-      <c r="C55" s="2">
-        <v>4</v>
-      </c>
-      <c r="D55" s="2">
-        <v>12</v>
-      </c>
-      <c r="E55" s="2">
-        <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="F55" s="2">
-        <v>1</v>
-      </c>
-      <c r="G55" s="2">
-        <v>1</v>
-      </c>
-      <c r="H55" s="2">
-        <v>0</v>
-      </c>
-      <c r="I55" s="2">
-        <v>6.9999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="2">
-        <v>9</v>
-      </c>
-      <c r="C56" s="2">
-        <v>2</v>
-      </c>
-      <c r="D56" s="2">
-        <v>9</v>
-      </c>
-      <c r="E56" s="2">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="F56" s="2">
-        <v>15</v>
-      </c>
-      <c r="G56" s="2">
-        <v>1</v>
-      </c>
-      <c r="H56" s="2">
-        <v>8</v>
-      </c>
-      <c r="I56" s="2">
-        <v>6.9999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B57" s="2">
-        <v>35</v>
       </c>
       <c r="C57" s="2">
         <v>4</v>
       </c>
       <c r="D57" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E57" s="2">
+        <v>2.8E-3</v>
+      </c>
+      <c r="F57" s="2">
+        <v>37</v>
+      </c>
+      <c r="G57" s="2">
+        <v>4</v>
+      </c>
+      <c r="H57" s="2">
+        <v>16</v>
+      </c>
+      <c r="I57" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="2">
+        <v>29</v>
+      </c>
+      <c r="C58" s="2">
+        <v>4</v>
+      </c>
+      <c r="D58" s="2">
+        <v>12</v>
+      </c>
+      <c r="E58" s="2">
         <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="F57" s="2">
-        <v>20</v>
-      </c>
-      <c r="G57" s="2">
-        <v>2</v>
-      </c>
-      <c r="H57" s="2">
-        <v>2</v>
-      </c>
-      <c r="I57" s="2">
-        <v>1.2999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B58" s="2">
-        <v>1</v>
-      </c>
-      <c r="C58" s="2">
-        <v>1</v>
-      </c>
-      <c r="D58" s="2">
-        <v>2</v>
-      </c>
-      <c r="E58" s="2">
-        <v>5.9999999999999995E-4</v>
       </c>
       <c r="F58" s="2">
         <v>1</v>
@@ -4071,75 +4353,164 @@
         <v>1</v>
       </c>
       <c r="H58" s="2">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="2">
+        <v>9</v>
+      </c>
+      <c r="C59" s="2">
         <v>2</v>
       </c>
-      <c r="I58" s="2">
+      <c r="D59" s="2">
+        <v>9</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="F59" s="2">
+        <v>15</v>
+      </c>
+      <c r="G59" s="2">
+        <v>1</v>
+      </c>
+      <c r="H59" s="2">
+        <v>8</v>
+      </c>
+      <c r="I59" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="2">
+        <v>35</v>
+      </c>
+      <c r="C60" s="2">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2">
+        <v>15</v>
+      </c>
+      <c r="E60" s="2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="F60" s="2">
+        <v>20</v>
+      </c>
+      <c r="G60" s="2">
+        <v>2</v>
+      </c>
+      <c r="H60" s="2">
+        <v>2</v>
+      </c>
+      <c r="I60" s="2">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2">
+        <v>2</v>
+      </c>
+      <c r="E61" s="2">
         <v>5.9999999999999995E-4</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="2" t="s">
+      <c r="F61" s="2">
+        <v>1</v>
+      </c>
+      <c r="G61" s="2">
+        <v>1</v>
+      </c>
+      <c r="H61" s="2">
+        <v>2</v>
+      </c>
+      <c r="I61" s="2">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B62" s="2">
         <v>0</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C62" s="2">
         <v>0</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D62" s="2">
         <v>0</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E62" s="2">
         <v>0</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F62" s="2">
         <v>0</v>
       </c>
-      <c r="G59" s="2">
+      <c r="G62" s="2">
         <v>0</v>
       </c>
-      <c r="H59" s="2">
+      <c r="H62" s="2">
         <v>0</v>
       </c>
-      <c r="I59" s="2">
+      <c r="I62" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="2" t="s">
+    <row r="63" spans="1:14">
+      <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B63" s="2">
         <v>23</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C63" s="2">
         <v>2</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D63" s="2">
         <v>12</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E63" s="2">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F63" s="2">
         <v>34</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G63" s="2">
         <v>3</v>
       </c>
-      <c r="H60" s="2">
+      <c r="H63" s="2">
         <v>13</v>
       </c>
-      <c r="I60" s="2">
+      <c r="I63" s="2">
         <v>1.8E-3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K53:N53"/>
+    <mergeCell ref="L4:O4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4153,11 +4524,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J53" sqref="J53:N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4170,27 +4541,32 @@
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="7.33203125" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1">
+      <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="30">
-      <c r="A2" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>53</v>
       </c>
@@ -4216,7 +4592,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4245,7 +4621,7 @@
         <v>5.6899999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4273,8 +4649,14 @@
       <c r="I4">
         <v>1.9300000000000001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="L4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4302,8 +4684,20 @@
       <c r="I5">
         <v>0.3785</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -4331,8 +4725,27 @@
       <c r="I6">
         <v>5.9400000000000001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="K6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="11">
+        <f>F54/B54</f>
+        <v>0.74257554302289686</v>
+      </c>
+      <c r="M6" s="11">
+        <f t="shared" ref="M6:O7" si="0">G54/C54</f>
+        <v>1.0077600671140938</v>
+      </c>
+      <c r="N6" s="11">
+        <f t="shared" si="0"/>
+        <v>1.006761073253833</v>
+      </c>
+      <c r="O6" s="11">
+        <f t="shared" si="0"/>
+        <v>0.99234162617282906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4360,8 +4773,27 @@
       <c r="I7">
         <v>3.8100000000000002E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="11">
+        <f>F55/B55</f>
+        <v>0.57873957436707046</v>
+      </c>
+      <c r="M7" s="11">
+        <f>G55/C55</f>
+        <v>1.0293237395645491</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0238893905450743</v>
+      </c>
+      <c r="O7" s="11">
+        <f t="shared" si="0"/>
+        <v>0.94945839688091427</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -4390,7 +4822,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4419,7 +4851,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4448,7 +4880,7 @@
         <v>5.3900000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -4477,7 +4909,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -4506,7 +4938,7 @@
         <v>2.1100000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -4535,7 +4967,7 @@
         <v>0.25109999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -4564,7 +4996,7 @@
         <v>0.1125</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -4593,7 +5025,7 @@
         <v>0.16830000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -5550,7 +5982,7 @@
         <v>0.18179999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -5579,7 +6011,7 @@
         <v>7.6799999999999993E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -5608,7 +6040,7 @@
         <v>2.9100000000000001E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -5637,7 +6069,7 @@
         <v>0.1825</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -5666,108 +6098,110 @@
         <v>6.5799999999999997E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="2" t="s">
+    <row r="53" spans="1:14">
+      <c r="B53" s="9"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="9">
+        <f>AVERAGE(B3:B52)</f>
+        <v>8163.56</v>
+      </c>
+      <c r="C54" s="9">
+        <f t="shared" ref="C54:I54" si="1">AVERAGE(C3:C52)</f>
+        <v>95.36</v>
+      </c>
+      <c r="D54" s="9">
+        <f t="shared" si="1"/>
+        <v>375.68</v>
+      </c>
+      <c r="E54" s="10">
+        <f t="shared" si="1"/>
+        <v>8.9313999999999977E-2</v>
+      </c>
+      <c r="F54" s="9">
+        <f t="shared" si="1"/>
+        <v>6062.06</v>
+      </c>
+      <c r="G54" s="9">
+        <f t="shared" si="1"/>
+        <v>96.1</v>
+      </c>
+      <c r="H54" s="9">
+        <f t="shared" si="1"/>
+        <v>378.22</v>
+      </c>
+      <c r="I54" s="10">
+        <f>AVERAGE(I3:I52)</f>
+        <v>8.8630000000000028E-2</v>
+      </c>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="9">
+        <f>_xlfn.STDEV.P(B3:B52)</f>
+        <v>16064.854043731613</v>
+      </c>
+      <c r="C55" s="9">
+        <f t="shared" ref="C55:I55" si="2">_xlfn.STDEV.P(C3:C52)</f>
+        <v>84.671071801412793</v>
+      </c>
+      <c r="D55" s="9">
+        <f t="shared" si="2"/>
+        <v>350.41406592772501</v>
+      </c>
+      <c r="E55" s="10">
+        <f t="shared" si="2"/>
+        <v>8.5354039178002591E-2</v>
+      </c>
+      <c r="F55" s="9">
+        <f t="shared" si="2"/>
+        <v>9297.3667915383448</v>
+      </c>
+      <c r="G55" s="9">
+        <f t="shared" si="2"/>
+        <v>87.153944259568661</v>
+      </c>
+      <c r="H55" s="9">
+        <f t="shared" si="2"/>
+        <v>358.78524440115984</v>
+      </c>
+      <c r="I55" s="10">
+        <f t="shared" si="2"/>
+        <v>8.1040109205257088E-2</v>
+      </c>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B57" s="2">
         <v>43</v>
-      </c>
-      <c r="C54" s="2">
-        <v>4</v>
-      </c>
-      <c r="D54" s="2">
-        <v>16</v>
-      </c>
-      <c r="E54" s="2">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="F54" s="2">
-        <v>35</v>
-      </c>
-      <c r="G54" s="2">
-        <v>4</v>
-      </c>
-      <c r="H54" s="2">
-        <v>16</v>
-      </c>
-      <c r="I54" s="2">
-        <v>2.3999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="2">
-        <v>29</v>
-      </c>
-      <c r="C55" s="2">
-        <v>4</v>
-      </c>
-      <c r="D55" s="2">
-        <v>12</v>
-      </c>
-      <c r="E55" s="2">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="F55" s="2">
-        <v>29</v>
-      </c>
-      <c r="G55" s="2">
-        <v>4</v>
-      </c>
-      <c r="H55" s="2">
-        <v>12</v>
-      </c>
-      <c r="I55" s="2">
-        <v>2.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="2">
-        <v>9</v>
-      </c>
-      <c r="C56" s="2">
-        <v>2</v>
-      </c>
-      <c r="D56" s="2">
-        <v>9</v>
-      </c>
-      <c r="E56" s="2">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="F56" s="2">
-        <v>9</v>
-      </c>
-      <c r="G56" s="2">
-        <v>2</v>
-      </c>
-      <c r="H56" s="2">
-        <v>9</v>
-      </c>
-      <c r="I56" s="2">
-        <v>1.1999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B57" s="2">
-        <v>35</v>
       </c>
       <c r="C57" s="2">
         <v>4</v>
       </c>
       <c r="D57" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E57" s="2">
-        <v>2.8999999999999998E-3</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="F57" s="2">
         <v>35</v>
@@ -5776,104 +6210,193 @@
         <v>4</v>
       </c>
       <c r="H57" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I57" s="2">
         <v>2.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:14">
       <c r="A58" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="2">
+        <v>29</v>
+      </c>
+      <c r="C58" s="2">
+        <v>4</v>
+      </c>
+      <c r="D58" s="2">
+        <v>12</v>
+      </c>
+      <c r="E58" s="2">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="F58" s="2">
+        <v>29</v>
+      </c>
+      <c r="G58" s="2">
+        <v>4</v>
+      </c>
+      <c r="H58" s="2">
+        <v>12</v>
+      </c>
+      <c r="I58" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="2">
+        <v>9</v>
+      </c>
+      <c r="C59" s="2">
+        <v>2</v>
+      </c>
+      <c r="D59" s="2">
+        <v>9</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="F59" s="2">
+        <v>9</v>
+      </c>
+      <c r="G59" s="2">
+        <v>2</v>
+      </c>
+      <c r="H59" s="2">
+        <v>9</v>
+      </c>
+      <c r="I59" s="2">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="2">
+        <v>35</v>
+      </c>
+      <c r="C60" s="2">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2">
+        <v>15</v>
+      </c>
+      <c r="E60" s="2">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="F60" s="2">
+        <v>35</v>
+      </c>
+      <c r="G60" s="2">
+        <v>4</v>
+      </c>
+      <c r="H60" s="2">
+        <v>15</v>
+      </c>
+      <c r="I60" s="2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B61" s="2">
         <v>1</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C61" s="2">
         <v>1</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D61" s="2">
         <v>2</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E61" s="2">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F61" s="2">
         <v>1</v>
       </c>
-      <c r="G58" s="2">
+      <c r="G61" s="2">
         <v>1</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H61" s="2">
         <v>2</v>
       </c>
-      <c r="I58" s="2">
+      <c r="I61" s="2">
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="2" t="s">
+    <row r="62" spans="1:14">
+      <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B62" s="2">
         <v>0</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C62" s="2">
         <v>0</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D62" s="2">
         <v>0</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E62" s="2">
         <v>1E-4</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F62" s="2">
         <v>0</v>
       </c>
-      <c r="G59" s="2">
+      <c r="G62" s="2">
         <v>0</v>
       </c>
-      <c r="H59" s="2">
+      <c r="H62" s="2">
         <v>0</v>
       </c>
-      <c r="I59" s="2">
+      <c r="I62" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="2" t="s">
+    <row r="63" spans="1:14">
+      <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B63" s="2">
         <v>23</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C63" s="2">
         <v>2</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D63" s="2">
         <v>12</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E63" s="2">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F63" s="2">
         <v>19</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G63" s="2">
         <v>2</v>
       </c>
-      <c r="H60" s="2">
+      <c r="H63" s="2">
         <v>12</v>
       </c>
-      <c r="I60" s="2">
+      <c r="I63" s="2">
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K53:N53"/>
+    <mergeCell ref="L4:O4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>